<commit_message>
2012 - NEW NAME SYSTEM
</commit_message>
<xml_diff>
--- a/Data/electrosamokaty/electrosamokat_2021_10.xlsx
+++ b/Data/electrosamokaty/electrosamokat_2021_10.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="375" windowWidth="27555" windowHeight="12045"/>
+    <workbookView xWindow="480" yWindow="380" windowWidth="17320" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -918,13 +919,13 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
-    <col min="3" max="3" width="58.7109375" customWidth="1"/>
-    <col min="12" max="14" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.1796875" customWidth="1"/>
+    <col min="3" max="3" width="58.7265625" customWidth="1"/>
+    <col min="12" max="14" width="15.26953125" customWidth="1"/>
     <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="21.42578125" customWidth="1"/>
+    <col min="19" max="19" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -9561,7 +9562,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9573,7 +9574,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>